<commit_message>
Update Employees.xlsx via Streamlit by Mohamed Abd El Ghany Omar
</commit_message>
<xml_diff>
--- a/Employees.xlsx
+++ b/Employees.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -639,6 +639,694 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>248</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Walaa Marie</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>36620537</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>01118022106</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>14</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>659</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mohamed Abdelhameid</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>36620538</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01061444247</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10001</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>663</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mohamed Refaat</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>36620539</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>01061444347</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>16</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10002</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1124</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fady Saied Ibrahim</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>36620540</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>01066254912</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>44958</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10003</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1751</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Peter Nagdy Fakry</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>36620541</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>01274938471</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="F11" t="n">
+        <v>18</v>
+      </c>
+      <c r="G11" t="n">
+        <v>10004</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1541</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Naglaa Ibrahim AbdElKader</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>36620542</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>01123823532</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45710</v>
+      </c>
+      <c r="F12" t="n">
+        <v>19</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10005</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>934</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Aghathon Loukas Mokhles</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>36620543</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>01279089941</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>44605</v>
+      </c>
+      <c r="F13" t="n">
+        <v>20</v>
+      </c>
+      <c r="G13" t="n">
+        <v>10006</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>657</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ahmed ibrahim Eissa</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>36620544</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>01030821888</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>21</v>
+      </c>
+      <c r="G14" t="n">
+        <v>10007</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>224</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Habiba Tarek</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>36620545</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>01112286918</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>22</v>
+      </c>
+      <c r="G15" t="n">
+        <v>10008</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>146</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Michael Ishaq</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>36620546</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>01277642246</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>23</v>
+      </c>
+      <c r="G16" t="n">
+        <v>10009</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>741</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Samer Samir Atallah</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>36620547</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>01118574998</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="F17" t="n">
+        <v>24</v>
+      </c>
+      <c r="G17" t="n">
+        <v>10010</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>721</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mina Adel Fouad</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>36620548</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>01030817555</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>44228</v>
+      </c>
+      <c r="F18" t="n">
+        <v>25</v>
+      </c>
+      <c r="G18" t="n">
+        <v>10011</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>932</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Mohamed ElSaid Metwally</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>36620549</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>01022257363</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>44604</v>
+      </c>
+      <c r="F19" t="n">
+        <v>26</v>
+      </c>
+      <c r="G19" t="n">
+        <v>10012</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1266</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Omar AbdelRahman Mousa</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>36620550</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>01060471962</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>45182</v>
+      </c>
+      <c r="F20" t="n">
+        <v>27</v>
+      </c>
+      <c r="G20" t="n">
+        <v>10013</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1035</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Nermeen Amin Khalil</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>36620551</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>01278844840</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>44913</v>
+      </c>
+      <c r="F21" t="n">
+        <v>28</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10014</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1614</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Dareen Hussein Ahmed</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>36620552</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>01027821333</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>45760</v>
+      </c>
+      <c r="F22" t="n">
+        <v>29</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10015</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>563</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Mohamed Enaya</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>36620553</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>01004846375</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>30</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10016</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>72</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Mostafa El Banna</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>36620554</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>01096958681</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>31</v>
+      </c>
+      <c r="G24" t="n">
+        <v>10017</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>945</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Khaled Ahmed AbdElGelil ElGendy</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>36620555</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>01020985077</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>44598</v>
+      </c>
+      <c r="F25" t="n">
+        <v>32</v>
+      </c>
+      <c r="G25" t="n">
+        <v>10018</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>968</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Abdallah Mohamed Mohamed Roshdy</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>36620556</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>01114000922</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>44699</v>
+      </c>
+      <c r="F26" t="n">
+        <v>33</v>
+      </c>
+      <c r="G26" t="n">
+        <v>10019</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Mohamed Sabry Ahmed</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>36620557</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>01021360024</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>44819</v>
+      </c>
+      <c r="F27" t="n">
+        <v>34</v>
+      </c>
+      <c r="G27" t="n">
+        <v>10020</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>884</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Islam Mohamed Elsayed</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>36620558</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>01063301935</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>44197</v>
+      </c>
+      <c r="F28" t="n">
+        <v>35</v>
+      </c>
+      <c r="G28" t="n">
+        <v>10021</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>